<commit_message>
Updated register test data
</commit_message>
<xml_diff>
--- a/src/main/resources/shoppingRegister.xlsx
+++ b/src/main/resources/shoppingRegister.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Input Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="21">
   <si>
     <t>male</t>
   </si>
@@ -27,38 +27,76 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>january</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
-    <t>california</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Home Address</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>12345678912</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>12346</t>
+  </si>
+  <si>
+    <t>email@ss.com5</t>
+  </si>
+  <si>
+    <t>email@ss.com6</t>
+  </si>
+  <si>
+    <t>email@ss.com7</t>
+  </si>
+  <si>
+    <t>email@ss.com8</t>
+  </si>
+  <si>
+    <t>email@ss.com9</t>
+  </si>
+  <si>
+    <t>email@ss.com10</t>
+  </si>
+  <si>
+    <t>email@ss.com11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="00000"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,14 +119,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,19 +429,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="13" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,20 +454,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>2000</v>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -435,24 +479,352 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1">
-        <v>7555555555</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1"/>
+    <hyperlink ref="D2:D3" r:id="rId2" display="email@ss.com5"/>
+    <hyperlink ref="D4" r:id="rId3" display="email@ss.com5"/>
+    <hyperlink ref="D7" r:id="rId4" display="email@ss.com5"/>
+    <hyperlink ref="D5:D6" r:id="rId5" display="email@ss.com5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added fail or pass to each row
</commit_message>
<xml_diff>
--- a/src/main/resources/shoppingRegister.xlsx
+++ b/src/main/resources/shoppingRegister.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="23">
   <si>
     <t>male</t>
   </si>
@@ -60,12 +60,6 @@
     <t>12346</t>
   </si>
   <si>
-    <t>email@ss.com5</t>
-  </si>
-  <si>
-    <t>email@ss.com6</t>
-  </si>
-  <si>
     <t>email@ss.com7</t>
   </si>
   <si>
@@ -75,10 +69,22 @@
     <t>email@ss.com9</t>
   </si>
   <si>
-    <t>email@ss.com10</t>
-  </si>
-  <si>
     <t>email@ss.com11</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>email@ss.com52</t>
+  </si>
+  <si>
+    <t>email@ss.com6455</t>
+  </si>
+  <si>
+    <t>email@ss.com101111</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +450,7 @@
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -496,8 +502,11 @@
       <c r="Q1" t="s">
         <v>5</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -508,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -549,8 +558,11 @@
       <c r="Q2" t="s">
         <v>5</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -561,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -602,8 +614,11 @@
       <c r="Q3" t="s">
         <v>5</v>
       </c>
+      <c r="R3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -614,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -655,8 +670,11 @@
       <c r="Q4" t="s">
         <v>5</v>
       </c>
+      <c r="R4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -667,7 +685,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -708,8 +726,11 @@
       <c r="Q5" t="s">
         <v>5</v>
       </c>
+      <c r="R5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -720,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -761,8 +782,11 @@
       <c r="Q6" t="s">
         <v>5</v>
       </c>
+      <c r="R6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -773,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -813,6 +837,9 @@
       </c>
       <c r="Q7" t="s">
         <v>5</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -822,9 +849,11 @@
     <hyperlink ref="D4" r:id="rId3" display="email@ss.com5"/>
     <hyperlink ref="D7" r:id="rId4" display="email@ss.com5"/>
     <hyperlink ref="D5:D6" r:id="rId5" display="email@ss.com5"/>
+    <hyperlink ref="D2" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>